<commit_message>
naar aanleiding van de feedback
</commit_message>
<xml_diff>
--- a/Modellen/Requirement architecture/constrance model.xlsx
+++ b/Modellen/Requirement architecture/constrance model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Themaopdracht6\Map tijdelijke documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Themaopdracht6\Modellen\Requirement architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>Verificatie</t>
   </si>
   <si>
-    <t>tempratuur sensor</t>
-  </si>
-  <si>
     <t>performance</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>user interface</t>
-  </si>
-  <si>
-    <t>tempratuur weergeven</t>
   </si>
   <si>
     <t>max 1 keer per seconde</t>
@@ -134,9 +128,6 @@
     <t>door te testen en te meten hoeveel hij gebruikt tijdens uitvoeren</t>
   </si>
   <si>
-    <t>snel en hoe vaak moet de tempratuur weergaven geüpdate worden</t>
-  </si>
-  <si>
     <t>meten hoe veel tijd er tussen updates zit.</t>
   </si>
   <si>
@@ -149,9 +140,6 @@
     <t>hoe lastig is het leren navigeren van de web interface</t>
   </si>
   <si>
-    <t>hoeveel de tempratuur sensor af mag wijken van de werkelijke temperatuur</t>
-  </si>
-  <si>
     <t>hoeveel procent mag het vullen van de wasmachine trommel afwijken</t>
   </si>
   <si>
@@ -168,6 +156,18 @@
   </si>
   <si>
     <t>door de sensor uit te lezen nadat er een bepaalde afgemeten hoeveelheid water in de trommel wordt gedaan.</t>
+  </si>
+  <si>
+    <t>temperatuur sensor</t>
+  </si>
+  <si>
+    <t>hoeveel de temperatuur sensor af mag wijken van de werkelijke temperatuur</t>
+  </si>
+  <si>
+    <t>temperatuur weergeven</t>
+  </si>
+  <si>
+    <t>snel en hoe vaak moet de temperatuur weergaven geüpdate worden</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -714,138 +714,138 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feedback verwerkt constrance model
</commit_message>
<xml_diff>
--- a/Modellen/Requirement architecture/constrance model.xlsx
+++ b/Modellen/Requirement architecture/constrance model.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Themaopdracht6\Modellen\Requirement architecture\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Identificatie</t>
   </si>
@@ -41,42 +36,21 @@
     <t>performance</t>
   </si>
   <si>
-    <t>hoeveel ram mag het gebruiken</t>
-  </si>
-  <si>
     <t>max 120 MB</t>
   </si>
   <si>
-    <t>user interface</t>
-  </si>
-  <si>
     <t>max 1 keer per seconde</t>
   </si>
   <si>
-    <t>vergrendelen WM deur</t>
-  </si>
-  <si>
     <t xml:space="preserve">water sensor </t>
   </si>
   <si>
-    <t>max 1%</t>
-  </si>
-  <si>
     <t>usability</t>
   </si>
   <si>
-    <t>de gebruiksvriendelijkheid van de UI</t>
-  </si>
-  <si>
     <t>resource use</t>
   </si>
   <si>
-    <t>learnability</t>
-  </si>
-  <si>
-    <t>learnability van de UI</t>
-  </si>
-  <si>
     <t>accuracy</t>
   </si>
   <si>
@@ -86,42 +60,9 @@
     <t>ram gebruik besturing WM</t>
   </si>
   <si>
-    <t>200 milliseconde</t>
-  </si>
-  <si>
-    <t>zonder gebruiksaanwijzing was kunnen starten</t>
-  </si>
-  <si>
     <t>door het na te meten met een geijkte thermometer</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">max 1 </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>o</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>C</t>
-    </r>
-  </si>
-  <si>
-    <t>door mensen buiten het development team te laten testen</t>
-  </si>
-  <si>
     <t>testen hoeveel acties er nodig zijn om een was te starten</t>
   </si>
   <si>
@@ -131,50 +72,44 @@
     <t>meten hoe veel tijd er tussen updates zit.</t>
   </si>
   <si>
-    <t>tijd die er tussen het geven van en uitvoeren van de deur vergrendeling mag zitten.</t>
-  </si>
-  <si>
-    <t>meten hoeveel tijd er tussen het versturen en het daadwekelijk vergrendelen zit</t>
-  </si>
-  <si>
-    <t>hoe lastig is het leren navigeren van de web interface</t>
-  </si>
-  <si>
-    <t>hoeveel procent mag het vullen van de wasmachine trommel afwijken</t>
-  </si>
-  <si>
     <t>3 - 4 muisklikken</t>
   </si>
   <si>
-    <t>door "Play tests" te doen en te kijken hoe veel moeite de gebruikers hebben</t>
-  </si>
-  <si>
-    <t>grote duidelijke knopen voor de hoofdtaken</t>
-  </si>
-  <si>
-    <t>hoe vaak moet de gebruiker klikken om een wasprogramma te starten</t>
-  </si>
-  <si>
     <t>door de sensor uit te lezen nadat er een bepaalde afgemeten hoeveelheid water in de trommel wordt gedaan.</t>
   </si>
   <si>
-    <t>temperatuur sensor</t>
-  </si>
-  <si>
-    <t>hoeveel de temperatuur sensor af mag wijken van de werkelijke temperatuur</t>
-  </si>
-  <si>
     <t>temperatuur weergeven</t>
   </si>
   <si>
-    <t>snel en hoe vaak moet de temperatuur weergaven geüpdate worden</t>
+    <t>temperatuur wasprogramma</t>
+  </si>
+  <si>
+    <t>hoeveel de temperatuur mag afwijken van de ingestelden temperatuur</t>
+  </si>
+  <si>
+    <t>max 1% ofwel hij mag er 1% onder zitten of 1% overheen zitten.</t>
+  </si>
+  <si>
+    <t>maximaal 3 oC erboven en eronder vanaf ingestelde temperatuur</t>
+  </si>
+  <si>
+    <t>hoeveel ram mag het wasprogramma op de raspberry pi gebruiken</t>
+  </si>
+  <si>
+    <t>Hoe snel en vaak moet de temperatuur weergaven geüpdate worden</t>
+  </si>
+  <si>
+    <t>het maximum aantal keer dat de gebruiker met de muis hoeft te klikken om in de goede volgorde het gewenste wasprogramma te starten</t>
+  </si>
+  <si>
+    <t>hoeveel procent mag het vullen van de wasmachine trommel afwijken van de ingestelde hoeveelheid van het gekozen wasprogramma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -182,13 +117,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -239,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -301,26 +229,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -353,21 +266,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -394,7 +292,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -436,7 +334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,10 +366,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,7 +400,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -679,14 +575,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -695,158 +591,128 @@
     <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" ht="25.5" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="51">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="E4" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="D5" s="10" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>34</v>
-      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -855,24 +721,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>